<commit_message>
second commit, no success
</commit_message>
<xml_diff>
--- a/TP_summary.xlsx
+++ b/TP_summary.xlsx
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1399218072289157</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -484,13 +484,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1540139</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0211575</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03141012048192771</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -510,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>9.300000000000001e-06</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -527,22 +527,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.03032120481927711</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.046</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>7.000000000000001e-07</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.30895507</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -553,22 +553,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.07805253012048192</v>
+        <v>0.1399218072289157</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1064433333333333</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1e-07</v>
+        <v>0.1540139</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.0211575</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -579,22 +579,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05993975903614458</v>
+        <v>0.03141012048192771</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1066075555555556</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>9.300000000000001e-06</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0211575</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -605,22 +605,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0907843373493976</v>
+        <v>0.03032120481927711</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05214155555555555</v>
+        <v>0.046</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>7.000000000000001e-07</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G7" t="n">
-        <v>0.28510611</v>
+        <v>0.30895507</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -631,22 +631,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.09285036144578313</v>
+        <v>0.07805253012048192</v>
       </c>
       <c r="C8" t="n">
-        <v>0.07308033333333333</v>
+        <v>0.1064433333333333</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1e-07</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04622738</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -657,10 +657,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.05457301204819277</v>
+        <v>0.05993975903614458</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.1066075555555556</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.0211575</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -683,22 +683,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1100657831325301</v>
+        <v>0.0907843373493976</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.05214155555555555</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1e-07</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.28510611</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -709,22 +709,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1024633734939759</v>
+        <v>0.09285036144578313</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.07308033333333333</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1e-07</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.04622738</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0601221686746988</v>
+        <v>0.05457301204819277</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0790119</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.08217590361445784</v>
+        <v>0.1100657831325301</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0522364</v>
+        <v>1e-07</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0973132530120482</v>
+        <v>0.1024633734939759</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1187736</v>
+        <v>1e-07</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -813,7 +813,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.03068361445783132</v>
+        <v>0.0601221686746988</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.0790119</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.04705325301204819</v>
+        <v>0.08217590361445784</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.0522364</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.05669566265060241</v>
+        <v>0.0973132530120482</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.1187736</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.01003771084337349</v>
+        <v>0.03068361445783132</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -917,7 +917,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.003303855421686747</v>
+        <v>0.04705325301204819</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -943,10 +943,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03396590361445783</v>
+        <v>0.05669566265060241</v>
       </c>
       <c r="C20" t="n">
-        <v>0.008888888888888889</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -969,10 +969,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.05506144578313253</v>
+        <v>0.01003771084337349</v>
       </c>
       <c r="C21" t="n">
-        <v>0.02444433333333333</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -995,10 +995,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.07964084337349397</v>
+        <v>0.003303855421686747</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0733228888888889</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -1021,10 +1021,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.05175807228915662</v>
+        <v>0.03396590361445783</v>
       </c>
       <c r="C23" t="n">
-        <v>0.03317822222222222</v>
+        <v>0.008888888888888889</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1047,10 +1047,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.02655518072289156</v>
+        <v>0.05506144578313253</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.02444433333333333</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1073,10 +1073,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.03576373493975903</v>
+        <v>0.07964084337349397</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.0733228888888889</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1099,10 +1099,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.04126951807228915</v>
+        <v>0.05175807228915662</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>0.03317822222222222</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.02239698795180723</v>
+        <v>0.02655518072289156</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -1151,10 +1151,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.05117216867469879</v>
+        <v>0.03576373493975903</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02222222222222222</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1177,7 +1177,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.006024096385542169</v>
+        <v>0.04126951807228915</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1203,7 +1203,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.006024096385542169</v>
+        <v>0.02239698795180723</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -1229,10 +1229,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.003012048192771084</v>
+        <v>0.05117216867469879</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1281,7 +1281,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -1307,7 +1307,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.004505783132530121</v>
+        <v>0.003012048192771084</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -1333,7 +1333,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.01356650602409639</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1359,7 +1359,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.006024096385542169</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1385,7 +1385,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>0.004505783132530121</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -1411,7 +1411,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0320855421686747</v>
+        <v>0.01356650602409639</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.02213132530120482</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -1463,7 +1463,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.01807228915662651</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -1489,7 +1489,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.006024096385542169</v>
+        <v>0.0320855421686747</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -1515,7 +1515,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0187821686746988</v>
+        <v>0.02213132530120482</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.01736240963855422</v>
+        <v>0.01807228915662651</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -1567,7 +1567,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.1473333333333333</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -1593,10 +1593,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.07578701904819278</v>
+        <v>0.0187821686746988</v>
       </c>
       <c r="C45" t="n">
-        <v>0.02867383512222222</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
@@ -1605,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.34758</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -1619,10 +1619,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.1061018266626506</v>
+        <v>0.01736240963855422</v>
       </c>
       <c r="C46" t="n">
-        <v>0.04014336917777778</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.29558</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -1645,10 +1645,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.1061018266626506</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>0.3331989247777778</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0.05066666666666667</v>
+        <v>0.1473333333333333</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
@@ -1671,10 +1671,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.1061018266626506</v>
+        <v>0.07578701904819278</v>
       </c>
       <c r="C48" t="n">
-        <v>0.450421147</v>
+        <v>0.02867383512222222</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.1003866666666667</v>
+        <v>0.34758</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -1697,10 +1697,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.1079155330963855</v>
+        <v>0.1061018266626506</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2794145758888888</v>
+        <v>0.04014336917777778</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -1709,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1703866666666667</v>
+        <v>0.29558</v>
       </c>
       <c r="G49" t="n">
-        <v>0.56858381</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -1723,10 +1723,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.1124497991927711</v>
+        <v>0.1061018266626506</v>
       </c>
       <c r="C50" t="n">
-        <v>0.05703703703333333</v>
+        <v>0.3331989247777778</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -1735,13 +1735,13 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>0.2513333333333334</v>
+        <v>0.05066666666666667</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0.09798285714285715</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1749,10 +1749,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.1124497991927711</v>
+        <v>0.1061018266626506</v>
       </c>
       <c r="C51" t="n">
-        <v>0.05703703703333333</v>
+        <v>0.450421147</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
@@ -1761,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1460577333333333</v>
+        <v>0.1003866666666667</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -1775,10 +1775,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.1124497991927711</v>
+        <v>0.1079155330963855</v>
       </c>
       <c r="C52" t="n">
-        <v>0.05703703703333333</v>
+        <v>0.2794145758888888</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -1787,10 +1787,10 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1703866666666667</v>
       </c>
       <c r="G52" t="n">
-        <v>0.31499264</v>
+        <v>0.56858381</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -1801,7 +1801,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.1865021060240964</v>
+        <v>0.1124497991927711</v>
       </c>
       <c r="C53" t="n">
         <v>0.05703703703333333</v>
@@ -1813,13 +1813,13 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.03</v>
+        <v>0.2513333333333334</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>0</v>
+        <v>0.09798285714285715</v>
       </c>
     </row>
     <row r="54">
@@ -1827,10 +1827,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.08639435791566265</v>
+        <v>0.1124497991927711</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>0.05703703703333333</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -1839,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.04</v>
+        <v>0.1460577333333333</v>
       </c>
       <c r="G54" t="n">
-        <v>0.40488609</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -1853,10 +1853,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.08639435791566265</v>
+        <v>0.1124497991927711</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>0.05703703703333333</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -1865,13 +1865,13 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>0.31499264</v>
       </c>
       <c r="H55" t="n">
-        <v>0.1365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1879,10 +1879,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.08639435791566265</v>
+        <v>0.1865021060240964</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>0.05703703703333333</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
@@ -1917,10 +1917,10 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G57" t="n">
-        <v>0</v>
+        <v>0.40488609</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -1946,10 +1946,10 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>0.13006082</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>0.1365</v>
       </c>
     </row>
     <row r="59">
@@ -1957,7 +1957,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>0.08639435791566265</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>0.14782203</v>
+        <v>0</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>0.08639435791566265</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
@@ -2009,7 +2009,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>0.08639435791566265</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>0.13006082</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -2047,10 +2047,10 @@
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>0.2106866666666667</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
+        <v>0.14782203</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>0.2106866666666667</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2165,10 +2165,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.07228915662650602</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.03555555555555556</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>0.048195</v>
+        <v>0</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
@@ -2191,10 +2191,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.08433734939759036</v>
+        <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.04148148147777778</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
@@ -2217,10 +2217,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.02409638554216868</v>
+        <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.01185185185555556</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
@@ -2243,10 +2243,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>0.07228915662650602</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="D70" t="n">
         <v>0</v>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>0.048195</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -2269,10 +2269,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>0.08433734939759036</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>0.04148148147777778</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
@@ -2295,10 +2295,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>0.02409638554216868</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>0.01185185185555556</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
@@ -2503,7 +2503,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.01204819277108434</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
@@ -2581,7 +2581,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>0.01204819277108434</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
@@ -2893,7 +2893,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.01993855421686747</v>
+        <v>0</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -2919,7 +2919,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.02221638554216868</v>
+        <v>0</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.02232469879518072</v>
+        <v>0</v>
       </c>
       <c r="C97" t="n">
         <v>0</v>
@@ -2971,7 +2971,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.001603734939759036</v>
+        <v>0.01993855421686747</v>
       </c>
       <c r="C98" t="n">
         <v>0</v>
@@ -2997,7 +2997,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.2701751807228916</v>
+        <v>0.02221638554216868</v>
       </c>
       <c r="C99" t="n">
         <v>0</v>
@@ -3006,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>0.1083260256</v>
+        <v>0</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -3023,7 +3023,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.6196668674698795</v>
+        <v>0.02232469879518072</v>
       </c>
       <c r="C100" t="n">
         <v>0</v>
@@ -3032,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>0.3028553624</v>
+        <v>0</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -3049,7 +3049,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.6074424096385542</v>
+        <v>0.001603734939759036</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0.3864837871</v>
+        <v>0</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -3075,7 +3075,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0</v>
+        <v>0.2701751807228916</v>
       </c>
       <c r="C102" t="n">
         <v>0</v>
@@ -3084,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>0</v>
+        <v>0.1083260256</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -3101,22 +3101,22 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.3023585542168675</v>
+        <v>0.6196668674698795</v>
       </c>
       <c r="C103" t="n">
-        <v>0.2096618357777778</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>0.4443478261</v>
+        <v>0.3028553624</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>0.739696</v>
+        <v>0</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -3127,16 +3127,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.4740856626506024</v>
+        <v>0.6074424096385542</v>
       </c>
       <c r="C104" t="n">
-        <v>0.2096618357777778</v>
+        <v>0</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>0.4443478261</v>
+        <v>0.3864837871</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -3153,16 +3153,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.689087108433735</v>
+        <v>0</v>
       </c>
       <c r="C105" t="n">
-        <v>0.2096618357777778</v>
+        <v>0</v>
       </c>
       <c r="D105" t="n">
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>0.4443478261</v>
+        <v>0</v>
       </c>
       <c r="F105" t="n">
         <v>0</v>
@@ -3179,25 +3179,25 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.2255324096385542</v>
+        <v>0.3023585542168675</v>
       </c>
       <c r="C106" t="n">
-        <v>0.05990338164444444</v>
+        <v>0.2096618357777778</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>0.1269565217</v>
+        <v>0.4443478261</v>
       </c>
       <c r="F106" t="n">
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>0</v>
+        <v>0.739696</v>
       </c>
       <c r="H106" t="n">
-        <v>0.07933714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -3205,22 +3205,22 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.01056072289156627</v>
+        <v>0.4740856626506024</v>
       </c>
       <c r="C107" t="n">
-        <v>0</v>
+        <v>0.2096618357777778</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>0.4443478261</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
       </c>
       <c r="G107" t="n">
-        <v>0.209831</v>
+        <v>0</v>
       </c>
       <c r="H107" t="n">
         <v>0</v>
@@ -3231,22 +3231,22 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.1460240963855422</v>
+        <v>0.689087108433735</v>
       </c>
       <c r="C108" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.2096618357777778</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>0.192</v>
+        <v>0.4443478261</v>
       </c>
       <c r="F108" t="n">
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -3257,25 +3257,25 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.2434043373493976</v>
+        <v>0.2255324096385542</v>
       </c>
       <c r="C109" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.05990338164444444</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>0.2428132</v>
+        <v>0.1269565217</v>
       </c>
       <c r="F109" t="n">
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>0.222411</v>
+        <v>0</v>
       </c>
       <c r="H109" t="n">
-        <v>0</v>
+        <v>0.07933714285714286</v>
       </c>
     </row>
     <row r="110">
@@ -3283,22 +3283,22 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.2571961445783132</v>
+        <v>0.01056072289156627</v>
       </c>
       <c r="C110" t="n">
-        <v>0.07333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>0.2454714</v>
+        <v>0</v>
       </c>
       <c r="F110" t="n">
         <v>0</v>
       </c>
       <c r="G110" t="n">
-        <v>0.367091</v>
+        <v>0.209831</v>
       </c>
       <c r="H110" t="n">
         <v>0</v>
@@ -3309,7 +3309,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.2625384338554217</v>
+        <v>0.1460240963855422</v>
       </c>
       <c r="C111" t="n">
         <v>0.07333333333333333</v>
@@ -3318,13 +3318,13 @@
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>0.2408561</v>
+        <v>0.192</v>
       </c>
       <c r="F111" t="n">
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -3335,7 +3335,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.2607413253012048</v>
+        <v>0.2434043373493976</v>
       </c>
       <c r="C112" t="n">
         <v>0.07333333333333333</v>
@@ -3344,13 +3344,13 @@
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>0.2388571</v>
+        <v>0.2428132</v>
       </c>
       <c r="F112" t="n">
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>0</v>
+        <v>0.222411</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -3361,25 +3361,25 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.004771807228915663</v>
+        <v>0.2571961445783132</v>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>0.2454714</v>
       </c>
       <c r="F113" t="n">
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>0</v>
+        <v>0.367091</v>
       </c>
       <c r="H113" t="n">
-        <v>0.2325085714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -3387,22 +3387,22 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.02390855421686747</v>
+        <v>0.2625384338554217</v>
       </c>
       <c r="C114" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>0.2408561</v>
       </c>
       <c r="F114" t="n">
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>0.065134</v>
+        <v>0</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -3413,16 +3413,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.01787385542168675</v>
+        <v>0.2607413253012048</v>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>0</v>
+        <v>0.2388571</v>
       </c>
       <c r="F115" t="n">
         <v>0</v>
@@ -3439,7 +3439,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>0.004771807228915663</v>
       </c>
       <c r="C116" t="n">
         <v>0</v>
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="H116" t="n">
-        <v>0</v>
+        <v>0.2325085714285714</v>
       </c>
     </row>
     <row r="117">
@@ -3465,7 +3465,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.007614457831325301</v>
+        <v>0.02390855421686747</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
@@ -3480,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>0</v>
+        <v>0.065134</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -3491,7 +3491,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0</v>
+        <v>0.01787385542168675</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
@@ -3543,7 +3543,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0</v>
+        <v>0.007614457831325301</v>
       </c>
       <c r="C120" t="n">
         <v>0</v>
@@ -3607,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>0.07083333333333333</v>
+        <v>0</v>
       </c>
       <c r="G122" t="n">
         <v>0</v>
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v>0.07083333333333333</v>
       </c>
       <c r="G125" t="n">
         <v>0</v>
@@ -3725,7 +3725,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.06855421685542168</v>
+        <v>0</v>
       </c>
       <c r="C127" t="n">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.1392151807228916</v>
+        <v>0</v>
       </c>
       <c r="C128" t="n">
         <v>0</v>
@@ -3777,7 +3777,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.1707351807228916</v>
+        <v>0</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -3803,7 +3803,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.2106519277108434</v>
+        <v>0.06855421685542168</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
@@ -3829,7 +3829,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0</v>
+        <v>0.1392151807228916</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -3855,7 +3855,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>0.1707351807228916</v>
       </c>
       <c r="C132" t="n">
         <v>0</v>
@@ -3881,7 +3881,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0</v>
+        <v>0.2106519277108434</v>
       </c>
       <c r="C133" t="n">
         <v>0</v>
@@ -4257,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="G147" t="n">
         <v>0</v>
@@ -4271,7 +4271,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.04719</v>
+        <v>0</v>
       </c>
       <c r="C148" t="n">
         <v>0</v>
@@ -4297,7 +4297,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.0165043373373494</v>
+        <v>0</v>
       </c>
       <c r="C149" t="n">
         <v>0</v>
@@ -4323,7 +4323,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.01464939759036145</v>
+        <v>0</v>
       </c>
       <c r="C150" t="n">
         <v>0</v>
@@ -4335,7 +4335,7 @@
         <v>0</v>
       </c>
       <c r="F150" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="G150" t="n">
         <v>0</v>
@@ -4349,7 +4349,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.01571518072289156</v>
+        <v>0.04719</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
@@ -4375,7 +4375,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.02003927710843374</v>
+        <v>0.0165043373373494</v>
       </c>
       <c r="C152" t="n">
         <v>0</v>
@@ -4401,7 +4401,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.01345</v>
+        <v>0.01464939759036145</v>
       </c>
       <c r="C153" t="n">
         <v>0</v>
@@ -4427,19 +4427,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.1646820484337349</v>
+        <v>0.01571518072289156</v>
       </c>
       <c r="C154" t="n">
-        <v>0.2106688888888889</v>
+        <v>0</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>0.11746637592</v>
+        <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>0.268</v>
+        <v>0</v>
       </c>
       <c r="G154" t="n">
         <v>0</v>
@@ -4453,22 +4453,22 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.3956048193975903</v>
+        <v>0.02003927710843374</v>
       </c>
       <c r="C155" t="n">
-        <v>0.2457803703333333</v>
+        <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>0.4057</v>
+        <v>0</v>
       </c>
       <c r="E155" t="n">
-        <v>0.3832896454</v>
+        <v>0</v>
       </c>
       <c r="F155" t="n">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G155" t="n">
-        <v>0.05684</v>
+        <v>0</v>
       </c>
       <c r="H155" t="n">
         <v>0</v>
@@ -4479,25 +4479,25 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.3978690361445783</v>
+        <v>0.01345</v>
       </c>
       <c r="C156" t="n">
-        <v>0.2457803703333333</v>
+        <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>0.4688666666666667</v>
+        <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>0.2937906507</v>
+        <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>0.28</v>
+        <v>0</v>
       </c>
       <c r="G156" t="n">
         <v>0</v>
       </c>
       <c r="H156" t="n">
-        <v>0.1314285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -4505,25 +4505,25 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.6633285543373494</v>
+        <v>0.1646820484337349</v>
       </c>
       <c r="C157" t="n">
-        <v>0.2457803703333333</v>
+        <v>0.2106688888888889</v>
       </c>
       <c r="D157" t="n">
-        <v>0.5917249999999999</v>
+        <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>0.51795569116</v>
+        <v>0.11746637592</v>
       </c>
       <c r="F157" t="n">
-        <v>0.14</v>
+        <v>0.268</v>
       </c>
       <c r="G157" t="n">
-        <v>0.528629</v>
+        <v>0</v>
       </c>
       <c r="H157" t="n">
-        <v>0.2442771428571429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -4531,25 +4531,25 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.3647754218072289</v>
+        <v>0.3956048193975903</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1053344444444445</v>
+        <v>0.2457803703333333</v>
       </c>
       <c r="D158" t="n">
-        <v>0.2841416666666667</v>
+        <v>0.4057</v>
       </c>
       <c r="E158" t="n">
-        <v>0.52578668083</v>
+        <v>0.3832896454</v>
       </c>
       <c r="F158" t="n">
-        <v>0.3782766666666666</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="G158" t="n">
-        <v>0</v>
+        <v>0.05684</v>
       </c>
       <c r="H158" t="n">
-        <v>0.3295514285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -4557,25 +4557,25 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0</v>
+        <v>0.3978690361445783</v>
       </c>
       <c r="C159" t="n">
-        <v>0</v>
+        <v>0.2457803703333333</v>
       </c>
       <c r="D159" t="n">
-        <v>0</v>
+        <v>0.4688666666666667</v>
       </c>
       <c r="E159" t="n">
-        <v>0</v>
+        <v>0.2937906507</v>
       </c>
       <c r="F159" t="n">
-        <v>0</v>
+        <v>0.28</v>
       </c>
       <c r="G159" t="n">
         <v>0</v>
       </c>
       <c r="H159" t="n">
-        <v>0</v>
+        <v>0.1314285714285714</v>
       </c>
     </row>
     <row r="160">
@@ -4583,25 +4583,25 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0</v>
+        <v>0.6633285543373494</v>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
+        <v>0.2457803703333333</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>0.5917249999999999</v>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>0.51795569116</v>
       </c>
       <c r="F160" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>0.528629</v>
       </c>
       <c r="H160" t="n">
-        <v>0</v>
+        <v>0.2442771428571429</v>
       </c>
     </row>
     <row r="161">
@@ -4609,25 +4609,25 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0</v>
+        <v>0.3647754218072289</v>
       </c>
       <c r="C161" t="n">
-        <v>0</v>
+        <v>0.1053344444444445</v>
       </c>
       <c r="D161" t="n">
-        <v>0</v>
+        <v>0.2841416666666667</v>
       </c>
       <c r="E161" t="n">
-        <v>0</v>
+        <v>0.52578668083</v>
       </c>
       <c r="F161" t="n">
-        <v>0</v>
+        <v>0.3782766666666666</v>
       </c>
       <c r="G161" t="n">
         <v>0</v>
       </c>
       <c r="H161" t="n">
-        <v>0</v>
+        <v>0.3295514285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed data and added stan features
</commit_message>
<xml_diff>
--- a/TP_summary.xlsx
+++ b/TP_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H161"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05117216867469879</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02222222222222222</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.006024096385542169</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.006024096385542169</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -631,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.003012048192771084</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -657,10 +657,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.006024096385542169</v>
+        <v>0.05117216867469879</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -709,7 +709,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.004505783132530121</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.01356650602409639</v>
+        <v>0.003012048192771084</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -813,7 +813,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.03208554216885542</v>
+        <v>0.004505783132530121</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.02213132530201205</v>
+        <v>0.01356650602409639</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0180722891566747</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.006024096385542169</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -917,7 +917,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0187821686746988</v>
+        <v>0.03208554216885542</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.01736240963855422</v>
+        <v>0.02213132530201205</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -969,7 +969,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>0.0180722891566747</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1473333333333333</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -995,10 +995,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.07578701904391566</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="C22" t="n">
-        <v>0.02867383512544444</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.34758</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1021,10 +1021,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1061018266614819</v>
+        <v>0.0187821686746988</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04014336917562222</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.29558</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1047,10 +1047,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1061018266614819</v>
+        <v>0.01736240963855422</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3331989247311778</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.05066666666666667</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1073,10 +1073,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1061018266614819</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4504211469534</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1003866666666667</v>
+        <v>0.1473333333333333</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1099,10 +1099,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1079155331001446</v>
+        <v>0.07578701904391566</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2794145758661889</v>
+        <v>0.02867383512544444</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1111,10 +1111,10 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1703866666666667</v>
+        <v>0.34758</v>
       </c>
       <c r="G26" t="n">
-        <v>0.56858381</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -1125,10 +1125,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1124497991967831</v>
+        <v>0.1061018266614819</v>
       </c>
       <c r="C27" t="n">
-        <v>0.05703703703703333</v>
+        <v>0.04014336917562222</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1137,13 +1137,13 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2513333333333334</v>
+        <v>0.29558</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0.09798285714285715</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1151,10 +1151,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1124497991967831</v>
+        <v>0.1061018266614819</v>
       </c>
       <c r="C28" t="n">
-        <v>0.05703703703703333</v>
+        <v>0.3331989247311778</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1460577333333333</v>
+        <v>0.05066666666666667</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1177,10 +1177,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1124497991967831</v>
+        <v>0.1061018266614819</v>
       </c>
       <c r="C29" t="n">
-        <v>0.05703703703703333</v>
+        <v>0.4504211469534</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1189,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1003866666666667</v>
       </c>
       <c r="G29" t="n">
-        <v>0.31499264</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1203,10 +1203,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1865021059849157</v>
+        <v>0.1079155331001446</v>
       </c>
       <c r="C30" t="n">
-        <v>0.05703703703703333</v>
+        <v>0.2794145758661889</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1215,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.03</v>
+        <v>0.1703866666666667</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>0.56858381</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1229,10 +1229,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.08639435791948193</v>
+        <v>0.1124497991967831</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.05703703703703333</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1241,13 +1241,13 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.04</v>
+        <v>0.2513333333333334</v>
       </c>
       <c r="G31" t="n">
-        <v>0.40488609</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>0.09798285714285715</v>
       </c>
     </row>
     <row r="32">
@@ -1255,10 +1255,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.08639435791948193</v>
+        <v>0.1124497991967831</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.05703703703703333</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -1267,13 +1267,13 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>0.1460577333333333</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.1365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1281,10 +1281,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.08639435791948193</v>
+        <v>0.1124497991967831</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.05703703703703333</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
@@ -1293,10 +1293,10 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.31499264</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1307,10 +1307,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.08639435791948193</v>
+        <v>0.1865021059849157</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.05703703703703333</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -1345,10 +1345,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G35" t="n">
-        <v>0.13006082</v>
+        <v>0.40488609</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -1359,7 +1359,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>0.08639435791948193</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1374,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0.14782203</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>0.1365</v>
       </c>
     </row>
     <row r="37">
@@ -1385,7 +1385,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>0.08639435791948193</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -1411,7 +1411,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>0.08639435791948193</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>0.08639435791948193</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -1449,10 +1449,10 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.2106866666666667</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>0.13006082</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>0.14782203</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>0.2106866666666667</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -1567,10 +1567,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.07228915662650602</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03555555555555556</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.048195</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -1593,10 +1593,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.08433734939759036</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0.04148148148147778</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
@@ -1619,10 +1619,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.02409638554216868</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.01185185185185556</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -1671,10 +1671,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>0.07228915662650602</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>0.048195</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -1697,10 +1697,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>0.08433734939759036</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>0.04148148148147778</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -1723,10 +1723,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>0.02409638554216868</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>0.01185185185185556</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -1905,7 +1905,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.01204819277108434</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -2009,7 +2009,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>0.01204819277108434</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
@@ -2295,7 +2295,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.01993855421686747</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
@@ -2321,7 +2321,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.02221638554216868</v>
+        <v>0</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
@@ -2347,7 +2347,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.02232469879518072</v>
+        <v>0</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
@@ -2373,7 +2373,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.001603734939759036</v>
+        <v>0</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
@@ -2399,10 +2399,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.2701751807590361</v>
+        <v>0.01993855421686747</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1203622506888889</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
@@ -2425,10 +2425,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.6196668674698795</v>
+        <v>0.02221638554216868</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3365059582111111</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
@@ -2451,10 +2451,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.6074424096265061</v>
+        <v>0.02232469879518072</v>
       </c>
       <c r="C78" t="n">
-        <v>0.4294264301333333</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
         <v>0</v>
@@ -2477,7 +2477,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>0.001603734939759036</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
@@ -2503,22 +2503,22 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.3023585542168675</v>
+        <v>0.2701751807590361</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2096618357487889</v>
+        <v>0.1203622506888889</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0.44434782608696</v>
+        <v>0</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.739696</v>
+        <v>0</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.474085662626506</v>
+        <v>0.6196668674698795</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2096618357487889</v>
+        <v>0.3365059582111111</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>0.44434782608696</v>
+        <v>0</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -2555,16 +2555,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.689087108433735</v>
+        <v>0.6074424096265061</v>
       </c>
       <c r="C82" t="n">
-        <v>0.2096618357487889</v>
+        <v>0.4294264301333333</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>0.44434782608696</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -2581,16 +2581,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.2255324096746988</v>
+        <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.05990338164251111</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>0.12695652173913</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="H83" t="n">
-        <v>0.07933714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2607,22 +2607,22 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.01056072289156627</v>
+        <v>0.3023585542168675</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>0.2096618357487889</v>
       </c>
       <c r="D84" t="n">
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>0.44434782608696</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0.209831</v>
+        <v>0.739696</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -2633,22 +2633,22 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.146024096373494</v>
+        <v>0.474085662626506</v>
       </c>
       <c r="C85" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.2096618357487889</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0.192</v>
+        <v>0.44434782608696</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -2659,22 +2659,22 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.243404337373494</v>
+        <v>0.689087108433735</v>
       </c>
       <c r="C86" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.2096618357487889</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>0.2428132</v>
+        <v>0.44434782608696</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0.222411</v>
+        <v>0</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -2685,25 +2685,25 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.2571961445783132</v>
+        <v>0.2255324096746988</v>
       </c>
       <c r="C87" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.05990338164251111</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0.2454714</v>
+        <v>0.12695652173913</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>0.367091</v>
+        <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>0.07933714285714286</v>
       </c>
     </row>
     <row r="88">
@@ -2711,22 +2711,22 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.2625384337951807</v>
+        <v>0.01056072289156627</v>
       </c>
       <c r="C88" t="n">
-        <v>0.07333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>0.2408561</v>
+        <v>0</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
+        <v>0.209831</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -2737,7 +2737,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.2607413253012048</v>
+        <v>0.146024096373494</v>
       </c>
       <c r="C89" t="n">
         <v>0.07333333333333333</v>
@@ -2746,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>0.2388571</v>
+        <v>0.192</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -2763,25 +2763,25 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.004771807228915663</v>
+        <v>0.243404337373494</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>1.93e-07</v>
+        <v>0.2428132</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>0.222411</v>
       </c>
       <c r="H90" t="n">
-        <v>0.2325085714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2789,22 +2789,22 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.02390855421686747</v>
+        <v>0.2571961445783132</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>0.2454714</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>0.065134</v>
+        <v>0.367091</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -2815,16 +2815,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.01787385542168675</v>
+        <v>0.2625384337951807</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>0.2408561</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -2841,16 +2841,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>0.2607413253012048</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>0.2388571</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -2867,7 +2867,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.007614457831325301</v>
+        <v>0.004771807228915663</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
@@ -2876,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>1.93e-07</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>0.2325085714285714</v>
       </c>
     </row>
     <row r="95">
@@ -2893,7 +2893,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>0.02390855421686747</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -2908,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>0.065134</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -2919,7 +2919,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>0.01787385542168675</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
@@ -2971,7 +2971,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>0.007614457831325301</v>
       </c>
       <c r="C98" t="n">
         <v>0</v>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>0.07083333333333333</v>
+        <v>0</v>
       </c>
       <c r="G99" t="n">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>0.07083333333333333</v>
       </c>
       <c r="G103" t="n">
         <v>0</v>
@@ -3127,7 +3127,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.06855421685542168</v>
+        <v>0</v>
       </c>
       <c r="C104" t="n">
         <v>0</v>
@@ -3153,7 +3153,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.1392151807469879</v>
+        <v>0</v>
       </c>
       <c r="C105" t="n">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.1707351807108434</v>
+        <v>0</v>
       </c>
       <c r="C106" t="n">
         <v>0</v>
@@ -3205,7 +3205,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.2106519277228916</v>
+        <v>0</v>
       </c>
       <c r="C107" t="n">
         <v>0</v>
@@ -3231,7 +3231,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>0.06855421685542168</v>
       </c>
       <c r="C108" t="n">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0</v>
+        <v>0.1392151807469879</v>
       </c>
       <c r="C109" t="n">
         <v>0</v>
@@ -3283,7 +3283,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0</v>
+        <v>0.1707351807108434</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
@@ -3309,7 +3309,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0</v>
+        <v>0.2106519277228916</v>
       </c>
       <c r="C111" t="n">
         <v>0</v>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="G124" t="n">
         <v>0</v>
@@ -3673,7 +3673,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.04719</v>
+        <v>0</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
@@ -3699,7 +3699,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.0165043373373494</v>
+        <v>0</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -3725,7 +3725,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.01464939759036145</v>
+        <v>0</v>
       </c>
       <c r="C127" t="n">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.01571518072289156</v>
+        <v>0</v>
       </c>
       <c r="C128" t="n">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="G128" t="n">
         <v>0</v>
@@ -3777,7 +3777,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.02003927710843374</v>
+        <v>0.04719</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -3803,7 +3803,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.01345</v>
+        <v>0.0165043373373494</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
@@ -3829,19 +3829,19 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.164682048373494</v>
+        <v>0.01464939759036145</v>
       </c>
       <c r="C131" t="n">
-        <v>0.3079203933222222</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>0.02994002193</v>
+        <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>0.268</v>
+        <v>0</v>
       </c>
       <c r="G131" t="n">
         <v>0</v>
@@ -3855,22 +3855,22 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.3956048193493976</v>
+        <v>0.01571518072289156</v>
       </c>
       <c r="C132" t="n">
-        <v>0.5309459808037</v>
+        <v>0</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>0.12664059604</v>
+        <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>0.05684</v>
+        <v>0</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -3881,25 +3881,25 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.3978690361566265</v>
+        <v>0.02003927710843374</v>
       </c>
       <c r="C133" t="n">
-        <v>0.5311395124036999</v>
+        <v>0</v>
       </c>
       <c r="D133" t="n">
-        <v>0.3614166666666667</v>
+        <v>0</v>
       </c>
       <c r="E133" t="n">
-        <v>0.0369674229</v>
+        <v>0</v>
       </c>
       <c r="F133" t="n">
-        <v>0.28</v>
+        <v>0</v>
       </c>
       <c r="G133" t="n">
         <v>0</v>
       </c>
       <c r="H133" t="n">
-        <v>0.1314285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -3907,25 +3907,25 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.663328554373494</v>
+        <v>0.01345</v>
       </c>
       <c r="C134" t="n">
-        <v>0.5309507692592556</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0.109275</v>
+        <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>0.26130233216</v>
+        <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>0.528629</v>
+        <v>0</v>
       </c>
       <c r="H134" t="n">
-        <v>0.2442771428571429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -3933,25 +3933,25 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.3647754218072289</v>
+        <v>0.164682048373494</v>
       </c>
       <c r="C135" t="n">
-        <v>0.2929468583666667</v>
+        <v>0.3079203933222222</v>
       </c>
       <c r="D135" t="n">
-        <v>0.2380916666666667</v>
+        <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>0.3569355082776</v>
+        <v>0.02994002193</v>
       </c>
       <c r="F135" t="n">
-        <v>0.3782766666666666</v>
+        <v>0.268</v>
       </c>
       <c r="G135" t="n">
         <v>0</v>
       </c>
       <c r="H135" t="n">
-        <v>0.3295514285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -3959,22 +3959,22 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0</v>
+        <v>0.3956048193493976</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1418370717333333</v>
+        <v>0.5309459808037</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>0.08126556325011</v>
+        <v>0.12664059604</v>
       </c>
       <c r="F136" t="n">
-        <v>0.14</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="G136" t="n">
-        <v>0</v>
+        <v>0.05684</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -3985,25 +3985,25 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0</v>
+        <v>0.3978690361566265</v>
       </c>
       <c r="C137" t="n">
-        <v>0</v>
+        <v>0.5311395124036999</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>0.3614166666666667</v>
       </c>
       <c r="E137" t="n">
-        <v>0.12025862254509</v>
+        <v>0.0369674229</v>
       </c>
       <c r="F137" t="n">
-        <v>0.1666666666667333</v>
+        <v>0.28</v>
       </c>
       <c r="G137" t="n">
-        <v>0.19941399999997</v>
+        <v>0</v>
       </c>
       <c r="H137" t="n">
-        <v>0.09180857142860001</v>
+        <v>0.1314285714285714</v>
       </c>
     </row>
     <row r="138">
@@ -4011,25 +4011,25 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0</v>
+        <v>0.663328554373494</v>
       </c>
       <c r="C138" t="n">
-        <v>0</v>
+        <v>0.5309507692592556</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>0.109275</v>
       </c>
       <c r="E138" t="n">
-        <v>0.13115204953986</v>
+        <v>0.26130233216</v>
       </c>
       <c r="F138" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G138" t="n">
-        <v>0.05684</v>
+        <v>0.528629</v>
       </c>
       <c r="H138" t="n">
-        <v>0.0881057142858</v>
+        <v>0.2442771428571429</v>
       </c>
     </row>
     <row r="139">
@@ -4037,25 +4037,25 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.0269722891686747</v>
+        <v>0.3647754218072289</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1694306501333333</v>
+        <v>0.2929468583666667</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>0.2380916666666667</v>
       </c>
       <c r="E139" t="n">
-        <v>0.13655231712391</v>
+        <v>0.3569355082776</v>
       </c>
       <c r="F139" t="n">
-        <v>0</v>
+        <v>0.3782766666666666</v>
       </c>
       <c r="G139" t="n">
         <v>0</v>
       </c>
       <c r="H139" t="n">
-        <v>0.0386428571428</v>
+        <v>0.3295514285714286</v>
       </c>
     </row>
     <row r="140">
@@ -4063,25 +4063,25 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.153542409626506</v>
+        <v>0</v>
       </c>
       <c r="C140" t="n">
-        <v>0.4198408069888889</v>
+        <v>0.1418370717333333</v>
       </c>
       <c r="D140" t="n">
-        <v>0.05951208333333333</v>
+        <v>0</v>
       </c>
       <c r="E140" t="n">
-        <v>0.23710104806911</v>
+        <v>0.08126556325011</v>
       </c>
       <c r="F140" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G140" t="n">
-        <v>0.20339999999998</v>
+        <v>0</v>
       </c>
       <c r="H140" t="n">
-        <v>0.0830857142858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -4089,25 +4089,25 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.3497124101686747</v>
+        <v>0</v>
       </c>
       <c r="C141" t="n">
-        <v>0.5284236113444445</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>0.08331691666666667</v>
+        <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>0.40056232752883</v>
+        <v>0.12025862254509</v>
       </c>
       <c r="F141" t="n">
-        <v>0</v>
+        <v>0.1666666666667333</v>
       </c>
       <c r="G141" t="n">
-        <v>0</v>
+        <v>0.19941399999997</v>
       </c>
       <c r="H141" t="n">
-        <v>0</v>
+        <v>0.09180857142860001</v>
       </c>
     </row>
     <row r="142">
@@ -4115,25 +4115,25 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.3526633735421686</v>
+        <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>0.3766591215444444</v>
+        <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>0.08331691666666667</v>
+        <v>0</v>
       </c>
       <c r="E142" t="n">
-        <v>0.39502810191749</v>
+        <v>0.13115204953986</v>
       </c>
       <c r="F142" t="n">
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>0.20340399999997</v>
+        <v>0.05684</v>
       </c>
       <c r="H142" t="n">
-        <v>0.19064</v>
+        <v>0.0881057142858</v>
       </c>
     </row>
     <row r="143">
@@ -4141,25 +4141,25 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.3590330122289156</v>
+        <v>0.0269722891686747</v>
       </c>
       <c r="C143" t="n">
-        <v>0.6552693410222222</v>
+        <v>0.1694306501333333</v>
       </c>
       <c r="D143" t="n">
-        <v>0.08331691666666667</v>
+        <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>0.40065604466512</v>
+        <v>0.13655231712391</v>
       </c>
       <c r="F143" t="n">
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>0.08249999999997</v>
+        <v>0</v>
       </c>
       <c r="H143" t="n">
-        <v>0</v>
+        <v>0.0386428571428</v>
       </c>
     </row>
     <row r="144">
@@ -4167,25 +4167,25 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.1842738554457831</v>
+        <v>0.153542409626506</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1615321619444444</v>
+        <v>0.4198408069888889</v>
       </c>
       <c r="D144" t="n">
-        <v>0.02380483333333333</v>
+        <v>0.05951208333333333</v>
       </c>
       <c r="E144" t="n">
-        <v>0.20305593256825</v>
+        <v>0.23710104806911</v>
       </c>
       <c r="F144" t="n">
-        <v>0.2106866666664667</v>
+        <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>0</v>
+        <v>0.20339999999998</v>
       </c>
       <c r="H144" t="n">
-        <v>0.0253314285714</v>
+        <v>0.0830857142858</v>
       </c>
     </row>
     <row r="145">
@@ -4193,16 +4193,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.1855016867228916</v>
+        <v>0.3497124101686747</v>
       </c>
       <c r="C145" t="n">
-        <v>0.06260175363333334</v>
+        <v>0.5284236113444445</v>
       </c>
       <c r="D145" t="n">
-        <v>0</v>
+        <v>0.08331691666666667</v>
       </c>
       <c r="E145" t="n">
-        <v>0.11693368472766</v>
+        <v>0.40056232752883</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="H145" t="n">
-        <v>0.0204257142858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -4219,25 +4219,25 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.07297987954216867</v>
+        <v>0.3526633735421686</v>
       </c>
       <c r="C146" t="n">
-        <v>0.06253945314444444</v>
+        <v>0.3766591215444444</v>
       </c>
       <c r="D146" t="n">
-        <v>0</v>
+        <v>0.08331691666666667</v>
       </c>
       <c r="E146" t="n">
-        <v>0.10872395601134</v>
+        <v>0.39502810191749</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
       </c>
       <c r="G146" t="n">
-        <v>0</v>
+        <v>0.20340399999997</v>
       </c>
       <c r="H146" t="n">
-        <v>0</v>
+        <v>0.19064</v>
       </c>
     </row>
     <row r="147">
@@ -4245,22 +4245,22 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.07791493975903614</v>
+        <v>0.3590330122289156</v>
       </c>
       <c r="C147" t="n">
-        <v>0.06240733366666667</v>
+        <v>0.6552693410222222</v>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>0.08331691666666667</v>
       </c>
       <c r="E147" t="n">
-        <v>0.10141199035604</v>
+        <v>0.40065604466512</v>
       </c>
       <c r="F147" t="n">
         <v>0</v>
       </c>
       <c r="G147" t="n">
-        <v>0</v>
+        <v>0.08249999999997</v>
       </c>
       <c r="H147" t="n">
         <v>0</v>
@@ -4271,25 +4271,25 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.03372746990361446</v>
+        <v>0.1842738554457831</v>
       </c>
       <c r="C148" t="n">
-        <v>0.03442158792222222</v>
+        <v>0.1615321619444444</v>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>0.02380483333333333</v>
       </c>
       <c r="E148" t="n">
-        <v>0.04211873454748</v>
+        <v>0.20305593256825</v>
       </c>
       <c r="F148" t="n">
-        <v>0</v>
+        <v>0.2106866666664667</v>
       </c>
       <c r="G148" t="n">
         <v>0</v>
       </c>
       <c r="H148" t="n">
-        <v>0</v>
+        <v>0.0253314285714</v>
       </c>
     </row>
     <row r="149">
@@ -4297,25 +4297,25 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0</v>
+        <v>0.1855016867228916</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>0.06260175363333334</v>
       </c>
       <c r="D149" t="n">
         <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>0.11693368472766</v>
       </c>
       <c r="F149" t="n">
-        <v>0.06264666666673334</v>
+        <v>0</v>
       </c>
       <c r="G149" t="n">
         <v>0</v>
       </c>
       <c r="H149" t="n">
-        <v>0</v>
+        <v>0.0204257142858</v>
       </c>
     </row>
     <row r="150">
@@ -4323,16 +4323,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>0.07297987954216867</v>
       </c>
       <c r="C150" t="n">
-        <v>0</v>
+        <v>0.06253945314444444</v>
       </c>
       <c r="D150" t="n">
         <v>0</v>
       </c>
       <c r="E150" t="n">
-        <v>0</v>
+        <v>0.10872395601134</v>
       </c>
       <c r="F150" t="n">
         <v>0</v>
@@ -4349,16 +4349,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0</v>
+        <v>0.07791493975903614</v>
       </c>
       <c r="C151" t="n">
-        <v>0</v>
+        <v>0.06240733366666667</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>0.10141199035604</v>
       </c>
       <c r="F151" t="n">
         <v>0</v>
@@ -4375,16 +4375,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0</v>
+        <v>0.03372746990361446</v>
       </c>
       <c r="C152" t="n">
-        <v>0</v>
+        <v>0.03442158792222222</v>
       </c>
       <c r="D152" t="n">
         <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>0.04211873454748</v>
       </c>
       <c r="F152" t="n">
         <v>0</v>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
+        <v>0.06264666666673334</v>
       </c>
       <c r="G153" t="n">
         <v>0</v>
@@ -4627,6 +4627,110 @@
         <v>0</v>
       </c>
       <c r="H161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0</v>
+      </c>
+      <c r="D162" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" t="n">
+        <v>0</v>
+      </c>
+      <c r="F162" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="n">
+        <v>0</v>
+      </c>
+      <c r="E163" t="n">
+        <v>0</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>0</v>
+      </c>
+      <c r="H163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0</v>
+      </c>
+      <c r="D164" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" t="n">
+        <v>0</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0</v>
+      </c>
+      <c r="G164" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0</v>
+      </c>
+      <c r="F165" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" t="n">
+        <v>0</v>
+      </c>
+      <c r="H165" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>